<commit_message>
Updated master sheets for PMC and PCMC
</commit_message>
<xml_diff>
--- a/input/pmc/Pune site mastersheet_3Nov21.xlsx
+++ b/input/pmc/Pune site mastersheet_3Nov21.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MP Ensystems\EVCI\Pune\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MP_Ensystem\Pune\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBC8570-4403-45E6-B5D5-E9DF01F62835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="5760" yWindow="2412" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMC OFFICE" sheetId="10" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="240">
   <si>
     <t>Narveer Tanaji Wadi, Shivajinagar, Pune, Maharashtra 411005</t>
   </si>
@@ -162,12 +163,6 @@
     <t>Shivajinagar, Pune, Maharashtra 411005</t>
   </si>
   <si>
-    <t>Chellaram Diabetes Hospital</t>
-  </si>
-  <si>
-    <t>1st Floor,, Lalani Quantum, Bavdhan Budruk, Pune, Maharashtra 411021</t>
-  </si>
-  <si>
     <t>Apollo Ct Scan Centre</t>
   </si>
   <si>
@@ -444,12 +439,6 @@
     <t>Jadhav Nagar, Mundhwa, Pune, Maharashtra 411028</t>
   </si>
   <si>
-    <t>Kasarwadi</t>
-  </si>
-  <si>
-    <t>Old Mumbai - Pune Hwy, Kasarwadi, Pimpri-Chinchwad, Maharashtra 411034</t>
-  </si>
-  <si>
     <t>S G S MALL</t>
   </si>
   <si>
@@ -480,12 +469,6 @@
     <t>Mahadji Shinde Rd, Near Parihar Chowk, Harmony Society, Ward No. 8, Wireless Colony, Aundh, Pune, Maharashtra 411007</t>
   </si>
   <si>
-    <t>Grand Highstreet</t>
-  </si>
-  <si>
-    <t>Phase 1, Hinjewadi Rajiv Gandhi Infotech Park, Hinjawadi, Pune, Maharashtra 411057</t>
-  </si>
-  <si>
     <t>Phoenix Marketcity - Viman Nagar</t>
   </si>
   <si>
@@ -525,9 +508,6 @@
     <t>Shivaji Road, Durvankur Society, Kasba Peth, Chhatrapati Shivaji Maharaj Rd, Pune, Maharashtra 411011</t>
   </si>
   <si>
-    <t>Balasaheb Thackeray Kaladalan</t>
-  </si>
-  <si>
     <t>Balgandrav Natyagruha</t>
   </si>
   <si>
@@ -579,15 +559,9 @@
     <t>EON Free Zone IT Park</t>
   </si>
   <si>
-    <t>SP Infocity IT Park</t>
-  </si>
-  <si>
     <t>Pune IT Park</t>
   </si>
   <si>
-    <t>Talawade IT Park</t>
-  </si>
-  <si>
     <t>ICC Tech Park</t>
   </si>
   <si>
@@ -684,9 +658,6 @@
     <t>Saras Baug, Pune, Maharashtra 411030</t>
   </si>
   <si>
-    <t>Pune, Maharashtra 412308</t>
-  </si>
-  <si>
     <t>Jhansi Rani Laxmibai Chowk, Shivajinagar, Pune, Maharashtra 411005</t>
   </si>
   <si>
@@ -708,27 +679,15 @@
     <t>Vitthal Rao Shivarkar Rd, Fatima Nagar, Wanowrie, Pune, Maharashtra 411010</t>
   </si>
   <si>
-    <t>Hinjewadi Rajiv Gandhi Infotech Park, Hinjawadi, Pimpri-Chinchwad, Maharashtra 411057</t>
-  </si>
-  <si>
-    <t>Hinjewadi Rajiv Gandhi Infotech Park</t>
-  </si>
-  <si>
     <t>Cybercity, Magarpatta, Hadapsar, Pune, Maharashtra 411013</t>
   </si>
   <si>
     <t>Eon Free Zone Rd, EON Free Zone, Kharadi, Pune, Maharashtra 411014</t>
   </si>
   <si>
-    <t>SP Infocity, Fursungi, Maharashtra 412308</t>
-  </si>
-  <si>
     <t>Bhau Patil Road, 34, Aundh Rd, Pragati Nagar, Marg, Pune, Maharashtra 411020</t>
   </si>
   <si>
-    <t>M I D C Technology Park, Talwade, Pimpri-Chinchwad, Maharashtra 411062</t>
-  </si>
-  <si>
     <t>Icc Tech Park 2, Senapati Bapat Rd, Laxmi Society, Model Colony, Shivajinagar, Pune, Maharashtra 411016</t>
   </si>
   <si>
@@ -775,13 +734,34 @@
   </si>
   <si>
     <t>College of Agriculture</t>
+  </si>
+  <si>
+    <t>Dr. Babasaheb Ambedkar Cantonment General Hospital</t>
+  </si>
+  <si>
+    <t>Bus Stop, Elphinston Road, Kasamali Jumbo Marg, Khadki, Pune, Maharashtra 411003</t>
+  </si>
+  <si>
+    <t>AFK HOCKEY GROUND</t>
+  </si>
+  <si>
+    <t>Khadki, Pune, Maharashtra 411003</t>
+  </si>
+  <si>
+    <t>Football Ground</t>
+  </si>
+  <si>
+    <t>Khadki Police Station</t>
+  </si>
+  <si>
+    <t>Pune Mumbai Highway, Church Chowk, Pune, Maharashtra 411003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,6 +913,12 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1279,7 +1265,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1336,6 +1322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1470,6 +1457,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1505,6 +1509,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1680,70 +1701,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="5">
+        <v>63</v>
+      </c>
+      <c r="D2">
         <v>73.85471579</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>18.524962550000001</v>
       </c>
       <c r="F2" s="8">
@@ -1761,20 +1782,20 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="5">
+        <v>65</v>
+      </c>
+      <c r="D3">
         <v>73.934007379999997</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>18.500346260000001</v>
       </c>
       <c r="F3" s="8">
@@ -1792,20 +1813,20 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="5">
+        <v>67</v>
+      </c>
+      <c r="D4">
         <v>73.854769509999997</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>18.50381325</v>
       </c>
       <c r="F4" s="8">
@@ -1821,49 +1842,49 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>73.839604429999994</v>
+      </c>
+      <c r="E5">
+        <v>18.512461500000001</v>
+      </c>
+      <c r="F5" s="8">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="5">
-        <v>73.839604429999994</v>
-      </c>
-      <c r="E5" s="5">
-        <v>18.512461500000001</v>
-      </c>
-      <c r="F5" s="8">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>73.852922000000007</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>18.52281</v>
       </c>
       <c r="F6" s="8">
@@ -1879,20 +1900,20 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="5">
+        <v>72</v>
+      </c>
+      <c r="D7">
         <v>73.845525440000003</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>18.524192410000001</v>
       </c>
       <c r="F7" s="8">
@@ -1908,20 +1929,20 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="5">
+        <v>74</v>
+      </c>
+      <c r="D8">
         <v>73.849691460000003</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>18.521934040000001</v>
       </c>
       <c r="F8" s="8">
@@ -1937,12 +1958,12 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I9" s="18">
         <v>270000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I10" s="19">
         <v>135000</v>
       </c>
@@ -1953,64 +1974,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D2">
         <v>73.908916026181203</v>
@@ -2037,64 +2059,65 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2">
         <v>73.874237043970297</v>
@@ -2115,12 +2138,12 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -2144,15 +2167,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4">
         <v>73.841116984440006</v>
@@ -2173,15 +2196,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>73.832818523163397</v>
@@ -2202,15 +2225,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6">
         <v>73.927813495426904</v>
@@ -2228,35 +2251,6 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7">
-        <v>73.821037702572397</v>
-      </c>
-      <c r="E7">
-        <v>18.607540540430001</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
         <v>270000</v>
       </c>
     </row>
@@ -2266,64 +2260,64 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D2" s="5">
         <v>73.877372599332801</v>
@@ -2344,15 +2338,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D3" s="5">
         <v>73.843328131677893</v>
@@ -2373,15 +2367,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D4" s="5">
         <v>73.838688257410297</v>
@@ -2402,15 +2396,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D5" s="5">
         <v>73.829760677582598</v>
@@ -2431,15 +2425,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" s="5">
         <v>73.806918644280898</v>
@@ -2460,21 +2454,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D7" s="5">
-        <v>73.725313563451806</v>
+        <v>73.916736997266497</v>
       </c>
       <c r="E7" s="5">
-        <v>18.594093063836699</v>
+        <v>18.562085545002802</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
@@ -2489,21 +2483,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D8" s="5">
-        <v>73.916736997266497</v>
+        <v>73.931283563809401</v>
       </c>
       <c r="E8" s="5">
-        <v>18.562085545002802</v>
+        <v>18.519627081675502</v>
       </c>
       <c r="F8" s="5">
         <v>5</v>
@@ -2518,21 +2512,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D9" s="5">
-        <v>73.931283563809401</v>
+        <v>73.934199637333194</v>
       </c>
       <c r="E9" s="5">
-        <v>18.519627081675502</v>
+        <v>18.518710583149101</v>
       </c>
       <c r="F9" s="5">
         <v>5</v>
@@ -2544,35 +2538,6 @@
         <v>1</v>
       </c>
       <c r="I9" s="5">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="5">
-        <v>73.934199637333194</v>
-      </c>
-      <c r="E10" s="5">
-        <v>18.518710583149101</v>
-      </c>
-      <c r="F10" s="5">
-        <v>5</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
         <v>270000</v>
       </c>
     </row>
@@ -2582,64 +2547,64 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D2">
         <v>73.855547506405898</v>
@@ -2660,15 +2625,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D3">
         <v>73.870524525125902</v>
@@ -2689,15 +2654,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D4">
         <v>73.853181226723805</v>
@@ -2718,15 +2683,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D5">
         <v>73.7631410189436</v>
@@ -2747,76 +2712,135 @@
         <v>270000</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6">
+        <v>73.857710142673696</v>
+      </c>
+      <c r="E6">
+        <v>18.5671418087144</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7">
+        <v>73.853135166450699</v>
+      </c>
+      <c r="E7">
+        <v>18.559916149772601</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>270000</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="6" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D2">
-        <v>73.964310634658304</v>
+        <v>73.848655205668194</v>
       </c>
       <c r="E2">
-        <v>18.462103475800799</v>
+        <v>18.521911868939998</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -2831,21 +2855,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D3">
-        <v>73.848655205668194</v>
+        <v>73.812626102565105</v>
       </c>
       <c r="E3">
-        <v>18.521911868939998</v>
+        <v>18.502822904944001</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -2860,21 +2884,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D4">
-        <v>73.812626102565105</v>
+        <v>73.867827173208795</v>
       </c>
       <c r="E4">
-        <v>18.502822904944001</v>
+        <v>18.525028689859301</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -2889,24 +2913,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D5">
-        <v>73.867827173208795</v>
+        <v>73.888503132295497</v>
       </c>
       <c r="E5">
-        <v>18.525028689859301</v>
+        <v>18.547874983016602</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2918,21 +2942,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D6">
-        <v>73.888503132295497</v>
+        <v>73.812977717784307</v>
       </c>
       <c r="E6">
-        <v>18.547874983016602</v>
+        <v>18.563157977944599</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -2947,21 +2971,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>221</v>
+        <v>161</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D7">
-        <v>73.812977717784307</v>
+        <v>73.899962696913207</v>
       </c>
       <c r="E7">
-        <v>18.563157977944599</v>
+        <v>18.497600164389802</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -2976,24 +3000,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D8">
-        <v>73.899962696913207</v>
+        <v>73.936570000000003</v>
       </c>
       <c r="E8">
-        <v>18.497600164389802</v>
+        <v>18.502939999999999</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3002,35 +3026,6 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D9">
-        <v>73.936570000000003</v>
-      </c>
-      <c r="E9">
-        <v>18.502939999999999</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
         <v>270000</v>
       </c>
     </row>
@@ -3041,72 +3036,72 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D2">
-        <v>73.731123884204393</v>
+        <v>73.925698905796494</v>
       </c>
       <c r="E2">
-        <v>18.594292038861099</v>
+        <v>18.5141296719545</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3117,26 +3112,25 @@
       <c r="I2" s="5">
         <v>270000</v>
       </c>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D3">
-        <v>73.925698905796494</v>
+        <v>73.950560453327</v>
       </c>
       <c r="E3">
-        <v>18.5141296719545</v>
+        <v>18.5509110046942</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3148,24 +3142,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D4">
-        <v>73.950560453327</v>
+        <v>73.831008858865303</v>
       </c>
       <c r="E4">
-        <v>18.5509110046942</v>
+        <v>18.566794316452601</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3177,21 +3171,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D5">
-        <v>73.951220258588506</v>
+        <v>73.829316588462902</v>
       </c>
       <c r="E5">
-        <v>18.488909479676401</v>
+        <v>18.531142075046098</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3206,21 +3200,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D6">
-        <v>73.831008858865303</v>
+        <v>73.910587546766493</v>
       </c>
       <c r="E6">
-        <v>18.566794316452601</v>
+        <v>18.544609732115902</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -3235,21 +3229,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D7">
-        <v>73.786891257529106</v>
+        <v>73.911764540425395</v>
       </c>
       <c r="E7">
-        <v>18.700431468079401</v>
+        <v>18.558906343488299</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -3264,24 +3258,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D8">
-        <v>73.829316588462902</v>
+        <v>73.919448720906402</v>
       </c>
       <c r="E8">
-        <v>18.531142075046098</v>
+        <v>18.563040277841399</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3293,24 +3287,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="D9">
-        <v>73.910587546766493</v>
+        <v>73.949252263651204</v>
       </c>
       <c r="E9">
-        <v>18.544609732115902</v>
+        <v>18.552698715305102</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3322,24 +3316,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D10">
-        <v>73.911764540425395</v>
+        <v>73.890510000000006</v>
       </c>
       <c r="E10">
-        <v>18.558906343488299</v>
+        <v>18.55058</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3351,24 +3345,24 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D11">
-        <v>73.919448720906402</v>
+        <v>73.927539999999993</v>
       </c>
       <c r="E11">
-        <v>18.563040277841399</v>
+        <v>18.5138</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3377,93 +3371,6 @@
         <v>1</v>
       </c>
       <c r="I11" s="5">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12">
-        <v>73.949252263651204</v>
-      </c>
-      <c r="E12">
-        <v>18.552698715305102</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D13">
-        <v>73.890510000000006</v>
-      </c>
-      <c r="E13">
-        <v>18.55058</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D14">
-        <v>73.927539999999993</v>
-      </c>
-      <c r="E14">
-        <v>18.5138</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5">
         <v>270000</v>
       </c>
     </row>
@@ -3474,62 +3381,62 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="5">
         <v>73.844130699999994</v>
@@ -3550,15 +3457,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="5">
         <v>73.856574899999998</v>
@@ -3579,15 +3486,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="5">
         <v>73.855131600000007</v>
@@ -3608,15 +3515,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="5">
         <v>73.880591100000004</v>
@@ -3637,15 +3544,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D6">
         <v>73.800469520919293</v>
@@ -3666,15 +3573,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D7">
         <v>73.767140652765207</v>
@@ -3695,15 +3602,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D8">
         <v>73.807431320247503</v>
@@ -3724,15 +3631,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D9">
         <v>73.788930993459203</v>
@@ -3759,69 +3666,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="14">
+        <v>76</v>
+      </c>
+      <c r="D2">
         <v>73.812989999999999</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2">
         <v>18.563170599999999</v>
       </c>
       <c r="F2" s="14">
@@ -3838,20 +3745,20 @@
       </c>
       <c r="J2" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="14">
+        <v>78</v>
+      </c>
+      <c r="D3">
         <v>73.887687799999995</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3">
         <v>18.545193600000001</v>
       </c>
       <c r="F3" s="14">
@@ -3868,20 +3775,20 @@
       </c>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="14">
+        <v>80</v>
+      </c>
+      <c r="D4">
         <v>73.9003096</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4">
         <v>18.503509000000001</v>
       </c>
       <c r="F4" s="14">
@@ -3898,50 +3805,50 @@
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <v>73.857860979999998</v>
+      </c>
+      <c r="E5">
+        <v>18.488972610000001</v>
+      </c>
+      <c r="F5" s="14">
+        <v>5</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>270000</v>
+      </c>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="14">
-        <v>73.857860979999998</v>
-      </c>
-      <c r="E5" s="14">
-        <v>18.488972610000001</v>
-      </c>
-      <c r="F5" s="14">
-        <v>5</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14">
-        <v>270000</v>
-      </c>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="14">
+      <c r="D6">
         <v>73.844327539999995</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6">
         <v>18.524041019999999</v>
       </c>
       <c r="F6" s="14">
@@ -3958,20 +3865,20 @@
       </c>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="14">
+        <v>82</v>
+      </c>
+      <c r="D7">
         <v>73.857922329999994</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7">
         <v>18.488978960000001</v>
       </c>
       <c r="F7" s="14">
@@ -3988,20 +3895,20 @@
       </c>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="14">
+        <v>87</v>
+      </c>
+      <c r="D8">
         <v>73.823631800000001</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8">
         <v>18.498284600000002</v>
       </c>
       <c r="F8" s="14">
@@ -4018,20 +3925,20 @@
       </c>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="14">
+        <v>89</v>
+      </c>
+      <c r="D9">
         <v>73.875711519999996</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9">
         <v>18.535842240000001</v>
       </c>
       <c r="F9" s="14">
@@ -4048,20 +3955,20 @@
       </c>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="14">
+        <v>91</v>
+      </c>
+      <c r="D10">
         <v>73.809325630000004</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10">
         <v>18.501184429999999</v>
       </c>
       <c r="F10" s="14">
@@ -4078,7 +3985,7 @@
       </c>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -4090,7 +3997,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -4109,57 +4016,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="30" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -4188,7 +4095,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -4217,7 +4124,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -4246,7 +4153,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -4275,7 +4182,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -4304,7 +4211,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -4333,7 +4240,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -4362,7 +4269,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -4391,7 +4298,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -4420,7 +4327,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -4449,7 +4356,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -4478,15 +4385,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="D13" s="11">
         <v>73.890630000000002</v>
@@ -4514,56 +4421,56 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4592,7 +4499,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4621,7 +4528,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -4650,7 +4557,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -4679,7 +4586,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -4693,65 +4600,65 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="21" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="14">
         <v>73.8705049</v>
@@ -4774,14 +4681,14 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="14">
@@ -4805,15 +4712,15 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="14">
         <v>73.858168399999997</v>
@@ -4836,15 +4743,15 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" s="14">
         <v>73.822496999999998</v>
@@ -4867,15 +4774,15 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" s="14">
         <v>73.828724399999999</v>
@@ -4898,15 +4805,15 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D7" s="14">
         <v>73.891551418724703</v>
@@ -4928,6 +4835,35 @@
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8">
+        <v>73.845314624229204</v>
+      </c>
+      <c r="E8">
+        <v>18.557168661678201</v>
+      </c>
+      <c r="F8" s="14">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14">
+        <v>270000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4936,56 +4872,56 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5014,7 +4950,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5043,7 +4979,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -5072,7 +5008,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5101,7 +5037,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -5112,10 +5048,10 @@
         <v>43</v>
       </c>
       <c r="D6" s="5">
-        <v>73.769805000000005</v>
+        <v>73.876533499999994</v>
       </c>
       <c r="E6" s="5">
-        <v>18.519442000000002</v>
+        <v>18.5303982</v>
       </c>
       <c r="F6" s="5">
         <v>5</v>
@@ -5130,7 +5066,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -5141,10 +5077,10 @@
         <v>45</v>
       </c>
       <c r="D7" s="5">
-        <v>73.876533499999994</v>
+        <v>73.786052900000001</v>
       </c>
       <c r="E7" s="5">
-        <v>18.5303982</v>
+        <v>18.564931399999999</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
@@ -5159,7 +5095,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -5170,10 +5106,10 @@
         <v>47</v>
       </c>
       <c r="D8" s="5">
-        <v>73.786052900000001</v>
+        <v>73.814811399999996</v>
       </c>
       <c r="E8" s="5">
-        <v>18.564931399999999</v>
+        <v>18.559656700000001</v>
       </c>
       <c r="F8" s="5">
         <v>5</v>
@@ -5188,7 +5124,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -5199,10 +5135,10 @@
         <v>49</v>
       </c>
       <c r="D9" s="5">
-        <v>73.814811399999996</v>
+        <v>73.871918100000002</v>
       </c>
       <c r="E9" s="5">
-        <v>18.559656700000001</v>
+        <v>18.5258529</v>
       </c>
       <c r="F9" s="5">
         <v>5</v>
@@ -5217,7 +5153,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -5228,10 +5164,10 @@
         <v>51</v>
       </c>
       <c r="D10" s="5">
-        <v>73.871918100000002</v>
+        <v>73.840964099999994</v>
       </c>
       <c r="E10" s="5">
-        <v>18.5258529</v>
+        <v>18.5011838</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
@@ -5246,21 +5182,21 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="5">
-        <v>73.840964099999994</v>
-      </c>
-      <c r="E11" s="5">
-        <v>18.5011838</v>
+      <c r="B11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11">
+        <v>73.848631938325497</v>
+      </c>
+      <c r="E11">
+        <v>18.568654349949998</v>
       </c>
       <c r="F11" s="5">
         <v>5</v>
@@ -5277,68 +5213,69 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D2" s="5">
         <v>73.860797155078799</v>
@@ -5359,15 +5296,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D3" s="5">
         <v>73.798256794741704</v>
@@ -5388,15 +5325,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D4" s="5">
         <v>73.853774882577298</v>
@@ -5417,15 +5354,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D5" s="5">
         <v>73.852231713666399</v>
@@ -5446,15 +5383,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D6" s="5">
         <v>73.836788544823904</v>
@@ -5475,15 +5412,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D7" s="5">
         <v>73.837868947453103</v>
@@ -5504,15 +5441,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D8" s="5">
         <v>73.882564665288896</v>
@@ -5533,15 +5470,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D9" s="5">
         <v>73.847146127833398</v>
@@ -5562,15 +5499,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D10" s="5">
         <v>73.862303833498999</v>
@@ -5591,15 +5528,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D11" s="5">
         <v>73.878090091624301</v>
@@ -5620,15 +5557,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D12">
         <v>73.897797868306498</v>
@@ -5655,64 +5592,65 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="34" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2">
         <v>73.901595700000001</v>
@@ -5733,15 +5671,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>73.847099299999996</v>
@@ -5762,15 +5700,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D4">
         <v>73.829987000000003</v>
@@ -5791,15 +5729,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D5">
         <v>73.844570700000006</v>
@@ -5820,15 +5758,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D6">
         <v>73.855670000000003</v>
@@ -5849,15 +5787,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D7">
         <v>73.857069999999993</v>
@@ -5884,64 +5822,64 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="5">
         <v>73.856555099999994</v>
@@ -5962,15 +5900,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="5">
         <v>73.846298000000004</v>
@@ -5991,15 +5929,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="5">
         <v>73.856401899999994</v>
@@ -6020,15 +5958,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="5">
         <v>73.854196599999995</v>
@@ -6049,15 +5987,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="5">
         <v>73.855920699999999</v>
@@ -6078,15 +6016,15 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="D7">
         <v>73.872559999999993</v>

</xml_diff>